<commit_message>
Published state of ETDataset on 1 June 2018
</commit_message>
<xml_diff>
--- a/nodes_source_analyses/agriculture/agriculture_geothermal.converter.xlsx
+++ b/nodes_source_analyses/agriculture/agriculture_geothermal.converter.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="27907"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10523"/>
   <workbookPr showInkAnnotation="0" codeName="ThisWorkbook" autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/dorinevandervlies/Projects/etdataset/nodes_source_analyses/agriculture/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/marliekeverweij/Projects/etdataset/nodes_source_analyses/agriculture/"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2F1F55C6-BE3D-8C40-A245-B10F1F35CCB0}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="27960" windowHeight="17540" tabRatio="762" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="27960" windowHeight="17540" tabRatio="762" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Cover sheet" sheetId="14" r:id="rId1"/>
@@ -36,7 +37,7 @@
     <definedName name="Wp_to_kWp">#REF!</definedName>
     <definedName name="WP_to_MWp">#REF!</definedName>
   </definedNames>
-  <calcPr calcId="150001" calcOnSave="0" concurrentCalc="0"/>
+  <calcPr calcId="179017" calcOnSave="0"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
       <x14:workbookPr defaultImageDpi="32767"/>
@@ -453,6 +454,7 @@
         <sz val="12"/>
         <color rgb="FF000000"/>
         <rFont val="Calibri"/>
+        <family val="2"/>
       </rPr>
       <t xml:space="preserve"> rake import:node NODE="nodename"</t>
     </r>
@@ -471,17 +473,24 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="2">
     <numFmt numFmtId="164" formatCode="0.0"/>
     <numFmt numFmtId="165" formatCode="0.000"/>
   </numFmts>
-  <fonts count="28" x14ac:knownFonts="1">
+  <fonts count="29">
     <font>
       <sz val="12"/>
       <color theme="1"/>
       <name val="Lettertype hoofdtekst"/>
       <family val="2"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
     <font>
       <sz val="12"/>
@@ -600,6 +609,7 @@
       <sz val="12"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -607,6 +617,7 @@
       <sz val="12"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -614,6 +625,7 @@
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -621,6 +633,7 @@
       <sz val="16"/>
       <color rgb="FF1F497D"/>
       <name val="Calibri"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -628,6 +641,7 @@
       <sz val="12"/>
       <color theme="10"/>
       <name val="Calibri"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -635,17 +649,20 @@
       <sz val="14"/>
       <color theme="1"/>
       <name val="Calibri"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="12"/>
       <name val="Calibri"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <b/>
       <sz val="12"/>
       <name val="Calibri"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -659,6 +676,7 @@
       <sz val="12"/>
       <color theme="1"/>
       <name val="Calibri"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -666,6 +684,7 @@
       <sz val="12"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="13">
@@ -1000,518 +1019,518 @@
   </borders>
   <cellStyleXfs count="253">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="top"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="153">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="16" fillId="2" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="17" fillId="2" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="2" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="17" fillId="2" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="5" xfId="177" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
-    <xf numFmtId="165" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="5" xfId="177" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="165" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="5" xfId="177" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
-    <xf numFmtId="0" fontId="17" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="5" xfId="177" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="18" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="19" fillId="3" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="18" fillId="3" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="20" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="18" fillId="3" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="3" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="18" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="17" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="17" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="17" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="17" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="17" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="17" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="14" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="17" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="17" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="18" fillId="3" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="17" fillId="3" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="19" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="17" fillId="3" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="3" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="17" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="16" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="16" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="16" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="16" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="18" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="14" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="21" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="14" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="19" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="17" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="16" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="16" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="13" fillId="2" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="13" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="16" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="16" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="17" fillId="3" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="17" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="13" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="20" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="13" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="18" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="16" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="2" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="12" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="12" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="12" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="12" fillId="2" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="12" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="12" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="12" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="12" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="22" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="22" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="2" fontId="12" fillId="2" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="12" fillId="2" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="13" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="13" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="13" fillId="2" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="13" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="13" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="13" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="13" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="23" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="49" fontId="23" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="23" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="23" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="23" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="23" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="23" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="13" fillId="2" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="13" fillId="2" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="24" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="49" fontId="24" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="24" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="24" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="24" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="24" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="25" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="25" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="24" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="24" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="23" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="23" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="23" fillId="2" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="24" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="24" fillId="2" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="23" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="24" fillId="2" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="25" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="25" fillId="2" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="24" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="23" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="24" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" indent="2"/>
     </xf>
-    <xf numFmtId="0" fontId="23" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="24" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="23" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="24" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="23" fillId="2" borderId="0" xfId="177" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="24" fillId="2" borderId="0" xfId="177" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="164" fontId="23" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="24" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" indent="2"/>
     </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="49" fontId="23" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="24" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="2" fontId="16" fillId="2" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="2" fontId="17" fillId="2" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="23" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="24" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="23" fillId="2" borderId="0" xfId="177" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
-    <xf numFmtId="0" fontId="23" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="24" fillId="2" borderId="0" xfId="177" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="24" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="12" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="11" fillId="2" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="17" fillId="2" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="10" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="17" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="10" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="27" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="10" fillId="2" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="16" fillId="2" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="9" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="16" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="9" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="26" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="9" fillId="2" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="9" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="9" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="9" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="9" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="9" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="9" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="9" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="9" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="9" fillId="12" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="16" fillId="2" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="18" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="12" fillId="2" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="17" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="2" fontId="12" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="12" fillId="2" borderId="20" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="12" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="22" fillId="2" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="12" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="1" fontId="16" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="10" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="10" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="10" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="10" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="10" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="10" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="10" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="10" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="10" fillId="12" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="17" fillId="2" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="19" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="13" fillId="2" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="18" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="13" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="13" fillId="2" borderId="20" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="13" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="23" fillId="2" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="13" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="1" fontId="17" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="2" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="17" fillId="2" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="7" fillId="2" borderId="20" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="164" fontId="8" fillId="2" borderId="20" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="2" fontId="7" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="2" fontId="7" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="2" fontId="8" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="8" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="1" fontId="7" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="1" fontId="8" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="165" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="165" fontId="8" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="165" fontId="7" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="165" fontId="8" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="10" fontId="7" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="10" fontId="8" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="center" indent="2"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="2" fontId="7" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="8" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="7" fillId="2" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="164" fontId="8" fillId="2" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="164" fontId="8" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="center" indent="2"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="center" indent="2"/>
     </xf>
-    <xf numFmtId="1" fontId="7" fillId="2" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="1" fontId="8" fillId="2" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="3" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="3" fontId="8" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="center" indent="2"/>
     </xf>
-    <xf numFmtId="3" fontId="7" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="3" fontId="8" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="center" indent="3"/>
     </xf>
-    <xf numFmtId="3" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="3" fontId="8" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="center" indent="3"/>
     </xf>
-    <xf numFmtId="2" fontId="7" fillId="2" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="2" fontId="8" fillId="2" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="2" fontId="7" fillId="2" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="8" fillId="2" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="8" fillId="2" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="8" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="7" fillId="2" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="7" fillId="2" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="7" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="7" fillId="2" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="164" fontId="8" fillId="2" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="16" fillId="2" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="16" fillId="2" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="25" fillId="4" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="17" fillId="2" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="17" fillId="2" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="26" fillId="4" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="25" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="26" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="25" fillId="4" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="26" fillId="4" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="25" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="26" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="25" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="26" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="25" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="26" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="25" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="26" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="25" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="26" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="25" fillId="4" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="26" fillId="4" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1776,6 +1795,9 @@
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
     </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
   </extLst>
 </styleSheet>
 </file>
@@ -1797,7 +1819,13 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="2" name="Picture 1"/>
+        <xdr:cNvPr id="2" name="Picture 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0400-000002000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -1835,7 +1863,13 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="3" name="Picture 2"/>
+        <xdr:cNvPr id="3" name="Picture 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0400-000003000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -2295,40 +2329,40 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <sheetPr codeName="Sheet1" enableFormatConditionsCalculation="0"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:C23"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.6640625" defaultRowHeight="16"/>
   <cols>
-    <col min="1" max="1" width="3.42578125" style="31" customWidth="1"/>
-    <col min="2" max="2" width="9.140625" style="23" customWidth="1"/>
-    <col min="3" max="3" width="44.140625" style="23" customWidth="1"/>
-    <col min="4" max="16384" width="10.7109375" style="23"/>
+    <col min="1" max="1" width="3.5" style="31" customWidth="1"/>
+    <col min="2" max="2" width="9.1640625" style="23" customWidth="1"/>
+    <col min="3" max="3" width="44.1640625" style="23" customWidth="1"/>
+    <col min="4" max="16384" width="10.6640625" style="23"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" s="29" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:3" s="29" customFormat="1">
       <c r="A1" s="27"/>
       <c r="B1" s="28"/>
       <c r="C1" s="28"/>
     </row>
-    <row r="2" spans="1:3" ht="21" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" ht="21">
       <c r="A2" s="7"/>
       <c r="B2" s="30" t="s">
         <v>16</v>
       </c>
       <c r="C2" s="30"/>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:3">
       <c r="A3" s="7"/>
       <c r="B3" s="14"/>
       <c r="C3" s="14"/>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:3">
       <c r="A4" s="7"/>
       <c r="B4" s="8" t="s">
         <v>17</v>
@@ -2337,7 +2371,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:3">
       <c r="A5" s="7"/>
       <c r="B5" s="10" t="s">
         <v>62</v>
@@ -2346,7 +2380,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:3">
       <c r="A6" s="7"/>
       <c r="B6" s="12" t="s">
         <v>19</v>
@@ -2355,29 +2389,29 @@
         <v>20</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:3">
       <c r="A7" s="7"/>
       <c r="B7" s="14"/>
       <c r="C7" s="14"/>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:3">
       <c r="A8" s="7"/>
       <c r="B8" s="14"/>
       <c r="C8" s="14"/>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:3">
       <c r="A9" s="7"/>
       <c r="B9" s="75" t="s">
         <v>63</v>
       </c>
       <c r="C9" s="76"/>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:3">
       <c r="A10" s="7"/>
       <c r="B10" s="77"/>
       <c r="C10" s="78"/>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:3">
       <c r="A11" s="7"/>
       <c r="B11" s="77" t="s">
         <v>64</v>
@@ -2386,33 +2420,33 @@
         <v>65</v>
       </c>
     </row>
-    <row r="12" spans="1:3" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:3" ht="17" thickBot="1">
       <c r="A12" s="7"/>
       <c r="B12" s="77"/>
       <c r="C12" s="20" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="13" spans="1:3" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:3" ht="17" thickBot="1">
       <c r="A13" s="7"/>
       <c r="B13" s="77"/>
       <c r="C13" s="80" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:3">
       <c r="A14" s="7"/>
       <c r="B14" s="77"/>
       <c r="C14" s="78" t="s">
         <v>68</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:3">
       <c r="A15" s="7"/>
       <c r="B15" s="77"/>
       <c r="C15" s="78"/>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:3">
       <c r="A16" s="7"/>
       <c r="B16" s="77" t="s">
         <v>69</v>
@@ -2421,49 +2455,49 @@
         <v>70</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:3">
       <c r="A17" s="7"/>
       <c r="B17" s="77"/>
       <c r="C17" s="82" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:3">
       <c r="A18" s="7"/>
       <c r="B18" s="77"/>
       <c r="C18" s="83" t="s">
         <v>72</v>
       </c>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:3">
       <c r="A19" s="7"/>
       <c r="B19" s="77"/>
       <c r="C19" s="84" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:3">
       <c r="A20" s="7"/>
       <c r="B20" s="85"/>
       <c r="C20" s="86" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:3">
       <c r="A21" s="7"/>
       <c r="B21" s="85"/>
       <c r="C21" s="87" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:3">
       <c r="A22" s="7"/>
       <c r="B22" s="85"/>
       <c r="C22" s="88" t="s">
         <v>76</v>
       </c>
     </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:3">
       <c r="B23" s="85"/>
       <c r="C23" s="89" t="s">
         <v>77</v>
@@ -2476,38 +2510,38 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <sheetPr codeName="Sheet2" enableFormatConditionsCalculation="0">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+  <sheetPr codeName="Sheet2">
     <tabColor rgb="FFFFFF00"/>
   </sheetPr>
   <dimension ref="B1:K34"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="G4" sqref="G4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.6640625" defaultRowHeight="16"/>
   <cols>
-    <col min="1" max="1" width="3.28515625" style="37" customWidth="1"/>
-    <col min="2" max="2" width="3.7109375" style="37" customWidth="1"/>
+    <col min="1" max="1" width="3.33203125" style="37" customWidth="1"/>
+    <col min="2" max="2" width="3.6640625" style="37" customWidth="1"/>
     <col min="3" max="3" width="46" style="37" customWidth="1"/>
-    <col min="4" max="4" width="12.7109375" style="37" customWidth="1"/>
-    <col min="5" max="5" width="17.42578125" style="37" customWidth="1"/>
-    <col min="6" max="6" width="4.5703125" style="37" customWidth="1"/>
+    <col min="4" max="4" width="12.6640625" style="37" customWidth="1"/>
+    <col min="5" max="5" width="17.5" style="37" customWidth="1"/>
+    <col min="6" max="6" width="4.5" style="37" customWidth="1"/>
     <col min="7" max="7" width="45" style="37" customWidth="1"/>
-    <col min="8" max="8" width="5.140625" style="37" customWidth="1"/>
-    <col min="9" max="9" width="51.42578125" style="37" customWidth="1"/>
-    <col min="10" max="10" width="5.42578125" style="37" customWidth="1"/>
-    <col min="11" max="16384" width="10.7109375" style="37"/>
+    <col min="8" max="8" width="5.1640625" style="37" customWidth="1"/>
+    <col min="9" max="9" width="51.5" style="37" customWidth="1"/>
+    <col min="10" max="10" width="5.5" style="37" customWidth="1"/>
+    <col min="11" max="16384" width="10.6640625" style="37"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:11" x14ac:dyDescent="0.2">
+    <row r="1" spans="2:11">
       <c r="D1" s="35"/>
       <c r="E1" s="35"/>
       <c r="F1" s="35"/>
       <c r="G1" s="35"/>
     </row>
-    <row r="2" spans="2:11" x14ac:dyDescent="0.2">
+    <row r="2" spans="2:11">
       <c r="B2" s="144" t="s">
         <v>120</v>
       </c>
@@ -2517,7 +2551,7 @@
       <c r="F2" s="35"/>
       <c r="G2" s="35"/>
     </row>
-    <row r="3" spans="2:11" x14ac:dyDescent="0.2">
+    <row r="3" spans="2:11">
       <c r="B3" s="147"/>
       <c r="C3" s="148"/>
       <c r="D3" s="148"/>
@@ -2525,7 +2559,7 @@
       <c r="F3" s="35"/>
       <c r="G3" s="35"/>
     </row>
-    <row r="4" spans="2:11" ht="34" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="2:11" ht="34" customHeight="1">
       <c r="B4" s="150"/>
       <c r="C4" s="151"/>
       <c r="D4" s="151"/>
@@ -2533,13 +2567,13 @@
       <c r="F4" s="35"/>
       <c r="G4" s="35"/>
     </row>
-    <row r="5" spans="2:11" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:11" ht="17" thickBot="1">
       <c r="D5" s="35"/>
       <c r="E5" s="35"/>
       <c r="F5" s="35"/>
       <c r="G5" s="35"/>
     </row>
-    <row r="6" spans="2:11" x14ac:dyDescent="0.2">
+    <row r="6" spans="2:11">
       <c r="B6" s="38"/>
       <c r="C6" s="22"/>
       <c r="D6" s="22"/>
@@ -2550,7 +2584,7 @@
       <c r="I6" s="22"/>
       <c r="J6" s="39"/>
     </row>
-    <row r="7" spans="2:11" s="44" customFormat="1" ht="19" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:11" s="44" customFormat="1" ht="19">
       <c r="B7" s="90"/>
       <c r="C7" s="21" t="s">
         <v>31</v>
@@ -2571,7 +2605,7 @@
       </c>
       <c r="J7" s="97"/>
     </row>
-    <row r="8" spans="2:11" s="44" customFormat="1" ht="19" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:11" s="44" customFormat="1" ht="19">
       <c r="B8" s="25"/>
       <c r="C8" s="20"/>
       <c r="D8" s="32"/>
@@ -2582,7 +2616,7 @@
       <c r="I8" s="20"/>
       <c r="J8" s="45"/>
     </row>
-    <row r="9" spans="2:11" s="44" customFormat="1" ht="20" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="2:11" s="44" customFormat="1" ht="20" thickBot="1">
       <c r="B9" s="25"/>
       <c r="C9" s="20" t="s">
         <v>89</v>
@@ -2595,7 +2629,7 @@
       <c r="I9" s="20"/>
       <c r="J9" s="45"/>
     </row>
-    <row r="10" spans="2:11" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="2:11" ht="17" thickBot="1">
       <c r="B10" s="40"/>
       <c r="C10" s="36" t="s">
         <v>33</v>
@@ -2615,7 +2649,7 @@
       <c r="J10" s="98"/>
       <c r="K10" s="35"/>
     </row>
-    <row r="11" spans="2:11" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="2:11" ht="17" thickBot="1">
       <c r="B11" s="40"/>
       <c r="C11" s="36" t="s">
         <v>35</v>
@@ -2635,7 +2669,7 @@
       <c r="J11" s="98"/>
       <c r="K11" s="35"/>
     </row>
-    <row r="12" spans="2:11" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="2:11" ht="17" thickBot="1">
       <c r="B12" s="40"/>
       <c r="C12" s="137" t="s">
         <v>98</v>
@@ -2655,7 +2689,7 @@
       <c r="J12" s="98"/>
       <c r="K12" s="35"/>
     </row>
-    <row r="13" spans="2:11" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="2:11" ht="17" thickBot="1">
       <c r="B13" s="40"/>
       <c r="C13" s="36" t="s">
         <v>10</v>
@@ -2675,7 +2709,7 @@
       <c r="J13" s="98"/>
       <c r="K13" s="35"/>
     </row>
-    <row r="14" spans="2:11" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="2:11" ht="17" thickBot="1">
       <c r="B14" s="40"/>
       <c r="C14" s="36" t="s">
         <v>37</v>
@@ -2695,7 +2729,7 @@
       <c r="J14" s="98"/>
       <c r="K14" s="35"/>
     </row>
-    <row r="15" spans="2:11" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="2:11" ht="17" thickBot="1">
       <c r="B15" s="40"/>
       <c r="C15" s="36" t="s">
         <v>38</v>
@@ -2715,7 +2749,7 @@
       <c r="J15" s="98"/>
       <c r="K15" s="35"/>
     </row>
-    <row r="16" spans="2:11" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="2:11" ht="17" thickBot="1">
       <c r="B16" s="40"/>
       <c r="C16" s="36" t="s">
         <v>39</v>
@@ -2736,7 +2770,7 @@
       </c>
       <c r="J16" s="98"/>
     </row>
-    <row r="17" spans="2:10" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:10" ht="17" thickBot="1">
       <c r="B17" s="40"/>
       <c r="C17" s="36" t="s">
         <v>40</v>
@@ -2758,7 +2792,7 @@
       </c>
       <c r="J17" s="98"/>
     </row>
-    <row r="18" spans="2:10" x14ac:dyDescent="0.2">
+    <row r="18" spans="2:10">
       <c r="B18" s="40"/>
       <c r="C18" s="73"/>
       <c r="D18" s="93"/>
@@ -2769,7 +2803,7 @@
       <c r="I18" s="35"/>
       <c r="J18" s="98"/>
     </row>
-    <row r="19" spans="2:10" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="2:10" ht="17" thickBot="1">
       <c r="B19" s="40"/>
       <c r="C19" s="20" t="s">
         <v>78</v>
@@ -2782,7 +2816,7 @@
       <c r="I19" s="35"/>
       <c r="J19" s="98"/>
     </row>
-    <row r="20" spans="2:10" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="2:10" ht="17" thickBot="1">
       <c r="B20" s="40"/>
       <c r="C20" s="36" t="s">
         <v>41</v>
@@ -2804,7 +2838,7 @@
       </c>
       <c r="J20" s="98"/>
     </row>
-    <row r="21" spans="2:10" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="2:10" ht="17" thickBot="1">
       <c r="B21" s="40"/>
       <c r="C21" s="36" t="s">
         <v>42</v>
@@ -2825,7 +2859,7 @@
       </c>
       <c r="J21" s="98"/>
     </row>
-    <row r="22" spans="2:10" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="2:10" ht="17" thickBot="1">
       <c r="B22" s="40"/>
       <c r="C22" s="36" t="s">
         <v>11</v>
@@ -2846,7 +2880,7 @@
       </c>
       <c r="J22" s="98"/>
     </row>
-    <row r="23" spans="2:10" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="2:10" ht="17" thickBot="1">
       <c r="B23" s="40"/>
       <c r="C23" s="36" t="s">
         <v>43</v>
@@ -2867,7 +2901,7 @@
       </c>
       <c r="J23" s="98"/>
     </row>
-    <row r="24" spans="2:10" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="2:10" ht="17" thickBot="1">
       <c r="B24" s="40"/>
       <c r="C24" s="36" t="s">
         <v>44</v>
@@ -2889,7 +2923,7 @@
       </c>
       <c r="J24" s="98"/>
     </row>
-    <row r="25" spans="2:10" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="2:10" ht="17" thickBot="1">
       <c r="B25" s="40"/>
       <c r="C25" s="36" t="s">
         <v>45</v>
@@ -2911,7 +2945,7 @@
       </c>
       <c r="J25" s="98"/>
     </row>
-    <row r="26" spans="2:10" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="2:10" ht="17" thickBot="1">
       <c r="B26" s="40"/>
       <c r="C26" s="36" t="s">
         <v>46</v>
@@ -2932,7 +2966,7 @@
       </c>
       <c r="J26" s="98"/>
     </row>
-    <row r="27" spans="2:10" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="2:10" ht="17" thickBot="1">
       <c r="B27" s="40"/>
       <c r="C27" s="36" t="s">
         <v>49</v>
@@ -2953,7 +2987,7 @@
       </c>
       <c r="J27" s="98"/>
     </row>
-    <row r="28" spans="2:10" x14ac:dyDescent="0.2">
+    <row r="28" spans="2:10">
       <c r="B28" s="40"/>
       <c r="C28" s="36"/>
       <c r="D28" s="24"/>
@@ -2964,7 +2998,7 @@
       <c r="I28" s="35"/>
       <c r="J28" s="98"/>
     </row>
-    <row r="29" spans="2:10" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="29" spans="2:10" ht="17" thickBot="1">
       <c r="B29" s="40"/>
       <c r="C29" s="20" t="s">
         <v>8</v>
@@ -2977,7 +3011,7 @@
       <c r="I29" s="35"/>
       <c r="J29" s="98"/>
     </row>
-    <row r="30" spans="2:10" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="30" spans="2:10" ht="17" thickBot="1">
       <c r="B30" s="40"/>
       <c r="C30" s="36" t="s">
         <v>36</v>
@@ -2998,7 +3032,7 @@
       </c>
       <c r="J30" s="98"/>
     </row>
-    <row r="31" spans="2:10" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="31" spans="2:10" ht="17" thickBot="1">
       <c r="B31" s="40"/>
       <c r="C31" s="36" t="s">
         <v>47</v>
@@ -3020,7 +3054,7 @@
       </c>
       <c r="J31" s="98"/>
     </row>
-    <row r="32" spans="2:10" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="32" spans="2:10" ht="17" thickBot="1">
       <c r="B32" s="40"/>
       <c r="C32" s="36" t="s">
         <v>48</v>
@@ -3042,7 +3076,7 @@
       </c>
       <c r="J32" s="98"/>
     </row>
-    <row r="33" spans="2:10" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="33" spans="2:10" ht="17" thickBot="1">
       <c r="B33" s="40"/>
       <c r="C33" s="36" t="s">
         <v>34</v>
@@ -3061,7 +3095,7 @@
       </c>
       <c r="J33" s="98"/>
     </row>
-    <row r="34" spans="2:10" ht="20" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="34" spans="2:10" ht="20" customHeight="1" thickBot="1">
       <c r="B34" s="41"/>
       <c r="C34" s="42"/>
       <c r="D34" s="42"/>
@@ -3082,35 +3116,35 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <sheetPr codeName="Sheet3" enableFormatConditionsCalculation="0">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+  <sheetPr codeName="Sheet3">
     <tabColor theme="6" tint="0.39997558519241921"/>
   </sheetPr>
   <dimension ref="B1:M19"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="F7" sqref="F7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.6640625" defaultRowHeight="16"/>
   <cols>
-    <col min="1" max="2" width="3.42578125" style="104" customWidth="1"/>
-    <col min="3" max="3" width="35.85546875" style="104" customWidth="1"/>
-    <col min="4" max="4" width="16.5703125" style="104" hidden="1" customWidth="1"/>
-    <col min="5" max="5" width="13.85546875" style="104" hidden="1" customWidth="1"/>
-    <col min="6" max="6" width="12.5703125" style="104" customWidth="1"/>
-    <col min="7" max="7" width="10.7109375" style="104" customWidth="1"/>
-    <col min="8" max="8" width="3.140625" style="104" customWidth="1"/>
-    <col min="9" max="9" width="8.42578125" style="105" customWidth="1"/>
-    <col min="10" max="10" width="2.42578125" style="105" customWidth="1"/>
-    <col min="11" max="11" width="8.5703125" style="105" customWidth="1"/>
+    <col min="1" max="2" width="3.5" style="104" customWidth="1"/>
+    <col min="3" max="3" width="35.83203125" style="104" customWidth="1"/>
+    <col min="4" max="4" width="16.5" style="104" hidden="1" customWidth="1"/>
+    <col min="5" max="5" width="13.83203125" style="104" hidden="1" customWidth="1"/>
+    <col min="6" max="6" width="12.5" style="104" customWidth="1"/>
+    <col min="7" max="7" width="10.6640625" style="104" customWidth="1"/>
+    <col min="8" max="8" width="3.1640625" style="104" customWidth="1"/>
+    <col min="9" max="9" width="8.5" style="105" customWidth="1"/>
+    <col min="10" max="10" width="2.5" style="105" customWidth="1"/>
+    <col min="11" max="11" width="8.5" style="105" customWidth="1"/>
     <col min="12" max="12" width="3" style="105" customWidth="1"/>
     <col min="13" max="13" width="60" style="104" customWidth="1"/>
-    <col min="14" max="16384" width="10.7109375" style="104"/>
+    <col min="14" max="16384" width="10.6640625" style="104"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:13" ht="17" thickBot="1" x14ac:dyDescent="0.25"/>
-    <row r="2" spans="2:13" x14ac:dyDescent="0.2">
+    <row r="1" spans="2:13" ht="17" thickBot="1"/>
+    <row r="2" spans="2:13">
       <c r="B2" s="106"/>
       <c r="C2" s="107"/>
       <c r="D2" s="107"/>
@@ -3124,7 +3158,7 @@
       <c r="L2" s="108"/>
       <c r="M2" s="109"/>
     </row>
-    <row r="3" spans="2:13" s="26" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="2:13" s="26" customFormat="1">
       <c r="B3" s="25"/>
       <c r="C3" s="100" t="s">
         <v>80</v>
@@ -3150,7 +3184,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="4" spans="2:13" x14ac:dyDescent="0.2">
+    <row r="4" spans="2:13">
       <c r="B4" s="110"/>
       <c r="C4" s="111"/>
       <c r="D4" s="111"/>
@@ -3164,7 +3198,7 @@
       <c r="L4" s="99"/>
       <c r="M4" s="2"/>
     </row>
-    <row r="5" spans="2:13" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:13" ht="17" thickBot="1">
       <c r="B5" s="110"/>
       <c r="C5" s="33" t="s">
         <v>79</v>
@@ -3180,7 +3214,7 @@
       <c r="L5" s="16"/>
       <c r="M5" s="3"/>
     </row>
-    <row r="6" spans="2:13" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:13" ht="17" thickBot="1">
       <c r="B6" s="110"/>
       <c r="C6" s="135" t="s">
         <v>91</v>
@@ -3204,7 +3238,7 @@
       <c r="L6" s="112"/>
       <c r="M6" s="3"/>
     </row>
-    <row r="7" spans="2:13" x14ac:dyDescent="0.2">
+    <row r="7" spans="2:13">
       <c r="B7" s="110"/>
       <c r="C7" s="115"/>
       <c r="D7" s="115"/>
@@ -3218,7 +3252,7 @@
       <c r="L7" s="117"/>
       <c r="M7" s="3"/>
     </row>
-    <row r="8" spans="2:13" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:13" ht="17" thickBot="1">
       <c r="B8" s="110"/>
       <c r="C8" s="33" t="s">
         <v>8</v>
@@ -3234,7 +3268,7 @@
       <c r="L8" s="116"/>
       <c r="M8" s="4"/>
     </row>
-    <row r="9" spans="2:13" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="2:13" ht="17" thickBot="1">
       <c r="B9" s="110"/>
       <c r="C9" s="119" t="s">
         <v>1</v>
@@ -3260,7 +3294,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="10" spans="2:13" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="2:13" ht="17" thickBot="1">
       <c r="B10" s="110"/>
       <c r="C10" s="120" t="s">
         <v>6</v>
@@ -3287,7 +3321,7 @@
       <c r="L10" s="116"/>
       <c r="M10" s="3"/>
     </row>
-    <row r="11" spans="2:13" x14ac:dyDescent="0.2">
+    <row r="11" spans="2:13">
       <c r="B11" s="110"/>
       <c r="C11" s="33"/>
       <c r="D11" s="33"/>
@@ -3301,7 +3335,7 @@
       <c r="L11" s="116"/>
       <c r="M11" s="3"/>
     </row>
-    <row r="12" spans="2:13" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="2:13" ht="17" thickBot="1">
       <c r="B12" s="110"/>
       <c r="C12" s="19" t="s">
         <v>81</v>
@@ -3317,7 +3351,7 @@
       <c r="L12" s="116"/>
       <c r="M12" s="3"/>
     </row>
-    <row r="13" spans="2:13" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="2:13" ht="17" thickBot="1">
       <c r="B13" s="110"/>
       <c r="C13" s="102" t="s">
         <v>82</v>
@@ -3338,7 +3372,7 @@
       <c r="L13" s="116"/>
       <c r="M13" s="3"/>
     </row>
-    <row r="14" spans="2:13" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="2:13" ht="17" thickBot="1">
       <c r="B14" s="110"/>
       <c r="C14" s="122" t="s">
         <v>9</v>
@@ -3361,7 +3395,7 @@
       <c r="L14" s="132"/>
       <c r="M14" s="3"/>
     </row>
-    <row r="15" spans="2:13" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="2:13" ht="17" thickBot="1">
       <c r="B15" s="110"/>
       <c r="C15" s="102" t="s">
         <v>83</v>
@@ -3382,7 +3416,7 @@
       <c r="L15" s="116"/>
       <c r="M15" s="3"/>
     </row>
-    <row r="16" spans="2:13" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="2:13" ht="17" thickBot="1">
       <c r="B16" s="110"/>
       <c r="C16" s="102" t="s">
         <v>84</v>
@@ -3405,7 +3439,7 @@
       <c r="L16" s="116"/>
       <c r="M16" s="3"/>
     </row>
-    <row r="17" spans="2:13" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:13" ht="17" thickBot="1">
       <c r="B17" s="110"/>
       <c r="C17" s="102" t="s">
         <v>85</v>
@@ -3425,7 +3459,7 @@
       <c r="L17" s="116"/>
       <c r="M17" s="3"/>
     </row>
-    <row r="18" spans="2:13" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="2:13" ht="17" thickBot="1">
       <c r="B18" s="110"/>
       <c r="C18" s="102" t="s">
         <v>85</v>
@@ -3445,7 +3479,7 @@
       <c r="L18" s="116"/>
       <c r="M18" s="4"/>
     </row>
-    <row r="19" spans="2:13" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="2:13" ht="17" thickBot="1">
       <c r="B19" s="126"/>
       <c r="C19" s="127"/>
       <c r="D19" s="127"/>
@@ -3466,8 +3500,8 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <sheetPr codeName="Sheet4" enableFormatConditionsCalculation="0">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
+  <sheetPr codeName="Sheet4">
     <tabColor theme="6" tint="0.79998168889431442"/>
   </sheetPr>
   <dimension ref="B1:K15"/>
@@ -3476,22 +3510,22 @@
       <selection activeCell="F13" sqref="F13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="33.140625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="33.1640625" defaultRowHeight="16"/>
   <cols>
-    <col min="1" max="1" width="3.28515625" style="48" customWidth="1"/>
-    <col min="2" max="2" width="3.42578125" style="48" customWidth="1"/>
-    <col min="3" max="3" width="28.7109375" style="48" customWidth="1"/>
-    <col min="4" max="4" width="3.140625" style="48" customWidth="1"/>
-    <col min="5" max="5" width="16.140625" style="48" customWidth="1"/>
-    <col min="6" max="6" width="10.28515625" style="48" customWidth="1"/>
-    <col min="7" max="9" width="12.140625" style="48" customWidth="1"/>
-    <col min="10" max="10" width="35.140625" style="49" customWidth="1"/>
-    <col min="11" max="11" width="60.42578125" style="48" customWidth="1"/>
-    <col min="12" max="16384" width="33.140625" style="48"/>
+    <col min="1" max="1" width="3.33203125" style="48" customWidth="1"/>
+    <col min="2" max="2" width="3.5" style="48" customWidth="1"/>
+    <col min="3" max="3" width="28.6640625" style="48" customWidth="1"/>
+    <col min="4" max="4" width="3.1640625" style="48" customWidth="1"/>
+    <col min="5" max="5" width="16.1640625" style="48" customWidth="1"/>
+    <col min="6" max="6" width="10.33203125" style="48" customWidth="1"/>
+    <col min="7" max="9" width="12.1640625" style="48" customWidth="1"/>
+    <col min="10" max="10" width="35.1640625" style="49" customWidth="1"/>
+    <col min="11" max="11" width="60.5" style="48" customWidth="1"/>
+    <col min="12" max="16384" width="33.1640625" style="48"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:11" ht="17" thickBot="1" x14ac:dyDescent="0.25"/>
-    <row r="2" spans="2:11" x14ac:dyDescent="0.2">
+    <row r="1" spans="2:11" ht="17" thickBot="1"/>
+    <row r="2" spans="2:11">
       <c r="B2" s="50"/>
       <c r="C2" s="51"/>
       <c r="D2" s="51"/>
@@ -3503,7 +3537,7 @@
       <c r="J2" s="52"/>
       <c r="K2" s="51"/>
     </row>
-    <row r="3" spans="2:11" x14ac:dyDescent="0.2">
+    <row r="3" spans="2:11">
       <c r="B3" s="53"/>
       <c r="C3" s="54" t="s">
         <v>21</v>
@@ -3517,7 +3551,7 @@
       <c r="J3" s="55"/>
       <c r="K3" s="56"/>
     </row>
-    <row r="4" spans="2:11" x14ac:dyDescent="0.2">
+    <row r="4" spans="2:11">
       <c r="B4" s="53"/>
       <c r="C4" s="56"/>
       <c r="D4" s="56"/>
@@ -3529,7 +3563,7 @@
       <c r="J4" s="57"/>
       <c r="K4" s="56"/>
     </row>
-    <row r="5" spans="2:11" x14ac:dyDescent="0.2">
+    <row r="5" spans="2:11">
       <c r="B5" s="58"/>
       <c r="C5" s="59" t="s">
         <v>29</v>
@@ -3557,7 +3591,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="6" spans="2:11" x14ac:dyDescent="0.2">
+    <row r="6" spans="2:11">
       <c r="B6" s="53"/>
       <c r="C6" s="54"/>
       <c r="D6" s="54"/>
@@ -3569,7 +3603,7 @@
       <c r="J6" s="55"/>
       <c r="K6" s="54"/>
     </row>
-    <row r="7" spans="2:11" x14ac:dyDescent="0.2">
+    <row r="7" spans="2:11">
       <c r="B7" s="53"/>
       <c r="C7" s="67"/>
       <c r="D7" s="61"/>
@@ -3593,7 +3627,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="8" spans="2:11" x14ac:dyDescent="0.2">
+    <row r="8" spans="2:11">
       <c r="B8" s="53"/>
       <c r="C8" s="62" t="s">
         <v>1</v>
@@ -3607,7 +3641,7 @@
       <c r="J8" s="57"/>
       <c r="K8" s="72"/>
     </row>
-    <row r="9" spans="2:11" x14ac:dyDescent="0.2">
+    <row r="9" spans="2:11">
       <c r="B9" s="53"/>
       <c r="C9" s="61" t="s">
         <v>61</v>
@@ -3621,7 +3655,7 @@
       <c r="J9" s="57"/>
       <c r="K9" s="72"/>
     </row>
-    <row r="10" spans="2:11" x14ac:dyDescent="0.2">
+    <row r="10" spans="2:11">
       <c r="B10" s="53"/>
       <c r="C10" s="66"/>
       <c r="D10" s="66"/>
@@ -3633,7 +3667,7 @@
       <c r="J10" s="64"/>
       <c r="K10" s="61"/>
     </row>
-    <row r="11" spans="2:11" x14ac:dyDescent="0.2">
+    <row r="11" spans="2:11">
       <c r="B11" s="53"/>
       <c r="C11" s="61"/>
       <c r="D11" s="61"/>
@@ -3657,7 +3691,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="12" spans="2:11" x14ac:dyDescent="0.2">
+    <row r="12" spans="2:11">
       <c r="B12" s="53"/>
       <c r="C12" s="62" t="s">
         <v>86</v>
@@ -3671,7 +3705,7 @@
       <c r="J12" s="68"/>
       <c r="K12" s="65"/>
     </row>
-    <row r="13" spans="2:11" x14ac:dyDescent="0.2">
+    <row r="13" spans="2:11">
       <c r="B13" s="53"/>
       <c r="C13" s="62" t="s">
         <v>96</v>
@@ -3685,7 +3719,7 @@
       <c r="J13" s="68"/>
       <c r="K13" s="61"/>
     </row>
-    <row r="14" spans="2:11" x14ac:dyDescent="0.2">
+    <row r="14" spans="2:11">
       <c r="B14" s="53"/>
       <c r="C14" s="62" t="s">
         <v>6</v>
@@ -3699,7 +3733,7 @@
       <c r="J14" s="68"/>
       <c r="K14" s="61"/>
     </row>
-    <row r="15" spans="2:11" x14ac:dyDescent="0.2">
+    <row r="15" spans="2:11">
       <c r="B15" s="53"/>
       <c r="C15" s="62" t="s">
         <v>112</v>
@@ -3723,24 +3757,24 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <sheetPr codeName="Sheet5" enableFormatConditionsCalculation="0"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
+  <sheetPr codeName="Sheet5"/>
   <dimension ref="B1:M50"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="M8" sqref="M8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.6640625" defaultRowHeight="16"/>
   <cols>
-    <col min="1" max="1" width="5.28515625" style="138" customWidth="1"/>
-    <col min="2" max="2" width="5.42578125" style="138" customWidth="1"/>
-    <col min="3" max="3" width="13.42578125" style="138" customWidth="1"/>
-    <col min="4" max="16384" width="10.7109375" style="138"/>
+    <col min="1" max="1" width="5.33203125" style="138" customWidth="1"/>
+    <col min="2" max="2" width="5.5" style="138" customWidth="1"/>
+    <col min="3" max="3" width="13.5" style="138" customWidth="1"/>
+    <col min="4" max="16384" width="10.6640625" style="138"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:13" ht="17" thickBot="1" x14ac:dyDescent="0.25"/>
-    <row r="2" spans="2:13" s="26" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="2:13" ht="17" thickBot="1"/>
+    <row r="2" spans="2:13" s="26" customFormat="1">
       <c r="B2" s="139"/>
       <c r="C2" s="140" t="s">
         <v>73</v>
@@ -3758,7 +3792,7 @@
       <c r="L2" s="140"/>
       <c r="M2" s="140"/>
     </row>
-    <row r="3" spans="2:13" x14ac:dyDescent="0.2">
+    <row r="3" spans="2:13">
       <c r="B3" s="141"/>
       <c r="C3" s="142"/>
       <c r="D3" s="142"/>
@@ -3772,7 +3806,7 @@
       <c r="L3" s="142"/>
       <c r="M3" s="142"/>
     </row>
-    <row r="4" spans="2:13" x14ac:dyDescent="0.2">
+    <row r="4" spans="2:13">
       <c r="B4" s="141"/>
       <c r="C4" s="142" t="s">
         <v>114</v>
@@ -3788,7 +3822,7 @@
       <c r="L4" s="142"/>
       <c r="M4" s="142"/>
     </row>
-    <row r="5" spans="2:13" x14ac:dyDescent="0.2">
+    <row r="5" spans="2:13">
       <c r="B5" s="141"/>
       <c r="C5" s="142" t="s">
         <v>101</v>
@@ -3804,7 +3838,7 @@
       <c r="L5" s="142"/>
       <c r="M5" s="142"/>
     </row>
-    <row r="6" spans="2:13" x14ac:dyDescent="0.2">
+    <row r="6" spans="2:13">
       <c r="B6" s="141"/>
       <c r="C6" s="142"/>
       <c r="D6" s="142"/>
@@ -3818,7 +3852,7 @@
       <c r="L6" s="142"/>
       <c r="M6" s="142"/>
     </row>
-    <row r="7" spans="2:13" x14ac:dyDescent="0.2">
+    <row r="7" spans="2:13">
       <c r="B7" s="141"/>
       <c r="C7" s="142"/>
       <c r="D7" s="142"/>
@@ -3832,7 +3866,7 @@
       <c r="L7" s="142"/>
       <c r="M7" s="142"/>
     </row>
-    <row r="8" spans="2:13" x14ac:dyDescent="0.2">
+    <row r="8" spans="2:13">
       <c r="B8" s="141"/>
       <c r="C8" s="142"/>
       <c r="D8" s="142"/>
@@ -3846,7 +3880,7 @@
       <c r="L8" s="142"/>
       <c r="M8" s="142"/>
     </row>
-    <row r="9" spans="2:13" x14ac:dyDescent="0.2">
+    <row r="9" spans="2:13">
       <c r="B9" s="141"/>
       <c r="C9" s="142"/>
       <c r="D9" s="142"/>
@@ -3860,7 +3894,7 @@
       <c r="L9" s="142"/>
       <c r="M9" s="142"/>
     </row>
-    <row r="10" spans="2:13" x14ac:dyDescent="0.2">
+    <row r="10" spans="2:13">
       <c r="B10" s="141"/>
       <c r="C10" s="142"/>
       <c r="D10" s="142"/>
@@ -3874,7 +3908,7 @@
       <c r="L10" s="142"/>
       <c r="M10" s="142"/>
     </row>
-    <row r="11" spans="2:13" x14ac:dyDescent="0.2">
+    <row r="11" spans="2:13">
       <c r="B11" s="141"/>
       <c r="C11" s="142"/>
       <c r="D11" s="142"/>
@@ -3888,7 +3922,7 @@
       <c r="L11" s="142"/>
       <c r="M11" s="142"/>
     </row>
-    <row r="12" spans="2:13" x14ac:dyDescent="0.2">
+    <row r="12" spans="2:13">
       <c r="B12" s="141"/>
       <c r="C12" s="142"/>
       <c r="D12" s="142"/>
@@ -3902,7 +3936,7 @@
       <c r="L12" s="142"/>
       <c r="M12" s="142"/>
     </row>
-    <row r="13" spans="2:13" x14ac:dyDescent="0.2">
+    <row r="13" spans="2:13">
       <c r="B13" s="141"/>
       <c r="C13" s="142"/>
       <c r="D13" s="142"/>
@@ -3916,7 +3950,7 @@
       <c r="L13" s="142"/>
       <c r="M13" s="142"/>
     </row>
-    <row r="14" spans="2:13" x14ac:dyDescent="0.2">
+    <row r="14" spans="2:13">
       <c r="B14" s="141"/>
       <c r="C14" s="142"/>
       <c r="D14" s="142"/>
@@ -3930,7 +3964,7 @@
       <c r="L14" s="142"/>
       <c r="M14" s="142"/>
     </row>
-    <row r="15" spans="2:13" x14ac:dyDescent="0.2">
+    <row r="15" spans="2:13">
       <c r="B15" s="141"/>
       <c r="C15" s="142"/>
       <c r="D15" s="142"/>
@@ -3944,7 +3978,7 @@
       <c r="L15" s="142"/>
       <c r="M15" s="142"/>
     </row>
-    <row r="16" spans="2:13" x14ac:dyDescent="0.2">
+    <row r="16" spans="2:13">
       <c r="B16" s="141"/>
       <c r="C16" s="142"/>
       <c r="D16" s="142"/>
@@ -3958,7 +3992,7 @@
       <c r="L16" s="142"/>
       <c r="M16" s="142"/>
     </row>
-    <row r="17" spans="2:13" x14ac:dyDescent="0.2">
+    <row r="17" spans="2:13">
       <c r="B17" s="141"/>
       <c r="C17" s="142"/>
       <c r="D17" s="142">
@@ -3976,7 +4010,7 @@
       <c r="L17" s="142"/>
       <c r="M17" s="142"/>
     </row>
-    <row r="18" spans="2:13" x14ac:dyDescent="0.2">
+    <row r="18" spans="2:13">
       <c r="B18" s="141"/>
       <c r="C18" s="142" t="s">
         <v>102</v>
@@ -3996,7 +4030,7 @@
       <c r="L18" s="142"/>
       <c r="M18" s="142"/>
     </row>
-    <row r="19" spans="2:13" x14ac:dyDescent="0.2">
+    <row r="19" spans="2:13">
       <c r="B19" s="141"/>
       <c r="C19" s="142" t="s">
         <v>104</v>
@@ -4016,7 +4050,7 @@
       <c r="L19" s="142"/>
       <c r="M19" s="142"/>
     </row>
-    <row r="20" spans="2:13" x14ac:dyDescent="0.2">
+    <row r="20" spans="2:13">
       <c r="B20" s="141"/>
       <c r="C20" s="142" t="s">
         <v>105</v>
@@ -4036,7 +4070,7 @@
       <c r="L20" s="142"/>
       <c r="M20" s="142"/>
     </row>
-    <row r="21" spans="2:13" x14ac:dyDescent="0.2">
+    <row r="21" spans="2:13">
       <c r="B21" s="141"/>
       <c r="C21" s="142"/>
       <c r="D21" s="142"/>
@@ -4050,7 +4084,7 @@
       <c r="L21" s="142"/>
       <c r="M21" s="142"/>
     </row>
-    <row r="22" spans="2:13" x14ac:dyDescent="0.2">
+    <row r="22" spans="2:13">
       <c r="B22" s="141"/>
       <c r="C22" s="142"/>
       <c r="D22" s="142"/>
@@ -4064,7 +4098,7 @@
       <c r="L22" s="142"/>
       <c r="M22" s="142"/>
     </row>
-    <row r="23" spans="2:13" x14ac:dyDescent="0.2">
+    <row r="23" spans="2:13">
       <c r="B23" s="141"/>
       <c r="C23" s="142"/>
       <c r="D23" s="142"/>
@@ -4078,7 +4112,7 @@
       <c r="L23" s="142"/>
       <c r="M23" s="142"/>
     </row>
-    <row r="24" spans="2:13" x14ac:dyDescent="0.2">
+    <row r="24" spans="2:13">
       <c r="B24" s="141"/>
       <c r="C24" s="142"/>
       <c r="D24" s="142"/>
@@ -4092,7 +4126,7 @@
       <c r="L24" s="142"/>
       <c r="M24" s="142"/>
     </row>
-    <row r="25" spans="2:13" x14ac:dyDescent="0.2">
+    <row r="25" spans="2:13">
       <c r="B25" s="141"/>
       <c r="C25" s="142"/>
       <c r="D25" s="142"/>
@@ -4106,7 +4140,7 @@
       <c r="L25" s="142"/>
       <c r="M25" s="142"/>
     </row>
-    <row r="26" spans="2:13" x14ac:dyDescent="0.2">
+    <row r="26" spans="2:13">
       <c r="B26" s="141"/>
       <c r="C26" s="142"/>
       <c r="D26" s="142"/>
@@ -4120,7 +4154,7 @@
       <c r="L26" s="142"/>
       <c r="M26" s="142"/>
     </row>
-    <row r="27" spans="2:13" x14ac:dyDescent="0.2">
+    <row r="27" spans="2:13">
       <c r="B27" s="141"/>
       <c r="C27" s="142"/>
       <c r="D27" s="142"/>
@@ -4134,7 +4168,7 @@
       <c r="L27" s="142"/>
       <c r="M27" s="142"/>
     </row>
-    <row r="28" spans="2:13" x14ac:dyDescent="0.2">
+    <row r="28" spans="2:13">
       <c r="B28" s="141"/>
       <c r="C28" s="142"/>
       <c r="D28" s="142"/>
@@ -4148,7 +4182,7 @@
       <c r="L28" s="142"/>
       <c r="M28" s="142"/>
     </row>
-    <row r="29" spans="2:13" x14ac:dyDescent="0.2">
+    <row r="29" spans="2:13">
       <c r="B29" s="141"/>
       <c r="C29" s="142"/>
       <c r="D29" s="142"/>
@@ -4162,7 +4196,7 @@
       <c r="L29" s="142"/>
       <c r="M29" s="142"/>
     </row>
-    <row r="30" spans="2:13" x14ac:dyDescent="0.2">
+    <row r="30" spans="2:13">
       <c r="B30" s="141"/>
       <c r="C30" s="142"/>
       <c r="D30" s="142"/>
@@ -4176,7 +4210,7 @@
       <c r="L30" s="142"/>
       <c r="M30" s="142"/>
     </row>
-    <row r="31" spans="2:13" x14ac:dyDescent="0.2">
+    <row r="31" spans="2:13">
       <c r="B31" s="141"/>
       <c r="C31" s="142" t="s">
         <v>93</v>
@@ -4192,7 +4226,7 @@
       <c r="L31" s="142"/>
       <c r="M31" s="142"/>
     </row>
-    <row r="32" spans="2:13" x14ac:dyDescent="0.2">
+    <row r="32" spans="2:13">
       <c r="B32" s="141"/>
       <c r="C32" s="142" t="s">
         <v>107</v>
@@ -4208,7 +4242,7 @@
       <c r="L32" s="142"/>
       <c r="M32" s="142"/>
     </row>
-    <row r="33" spans="2:13" x14ac:dyDescent="0.2">
+    <row r="33" spans="2:13">
       <c r="B33" s="141"/>
       <c r="C33" s="142"/>
       <c r="D33" s="142"/>
@@ -4222,7 +4256,7 @@
       <c r="L33" s="142"/>
       <c r="M33" s="142"/>
     </row>
-    <row r="34" spans="2:13" x14ac:dyDescent="0.2">
+    <row r="34" spans="2:13">
       <c r="B34" s="141"/>
       <c r="C34" s="142"/>
       <c r="D34" s="142"/>
@@ -4236,7 +4270,7 @@
       <c r="L34" s="142"/>
       <c r="M34" s="142"/>
     </row>
-    <row r="35" spans="2:13" x14ac:dyDescent="0.2">
+    <row r="35" spans="2:13">
       <c r="B35" s="141"/>
       <c r="C35" s="142"/>
       <c r="D35" s="142"/>
@@ -4250,7 +4284,7 @@
       <c r="L35" s="142"/>
       <c r="M35" s="142"/>
     </row>
-    <row r="36" spans="2:13" x14ac:dyDescent="0.2">
+    <row r="36" spans="2:13">
       <c r="B36" s="141"/>
       <c r="C36" s="142"/>
       <c r="D36" s="142"/>
@@ -4264,7 +4298,7 @@
       <c r="L36" s="142"/>
       <c r="M36" s="142"/>
     </row>
-    <row r="37" spans="2:13" x14ac:dyDescent="0.2">
+    <row r="37" spans="2:13">
       <c r="B37" s="141"/>
       <c r="C37" s="142"/>
       <c r="D37" s="142"/>
@@ -4278,7 +4312,7 @@
       <c r="L37" s="142"/>
       <c r="M37" s="142"/>
     </row>
-    <row r="38" spans="2:13" x14ac:dyDescent="0.2">
+    <row r="38" spans="2:13">
       <c r="B38" s="141"/>
       <c r="C38" s="142"/>
       <c r="D38" s="142"/>
@@ -4292,7 +4326,7 @@
       <c r="L38" s="142"/>
       <c r="M38" s="142"/>
     </row>
-    <row r="39" spans="2:13" x14ac:dyDescent="0.2">
+    <row r="39" spans="2:13">
       <c r="B39" s="141"/>
       <c r="C39" s="142"/>
       <c r="D39" s="142"/>
@@ -4306,7 +4340,7 @@
       <c r="L39" s="142"/>
       <c r="M39" s="142"/>
     </row>
-    <row r="40" spans="2:13" x14ac:dyDescent="0.2">
+    <row r="40" spans="2:13">
       <c r="B40" s="141"/>
       <c r="C40" s="142"/>
       <c r="D40" s="142"/>
@@ -4320,7 +4354,7 @@
       <c r="L40" s="142"/>
       <c r="M40" s="142"/>
     </row>
-    <row r="41" spans="2:13" x14ac:dyDescent="0.2">
+    <row r="41" spans="2:13">
       <c r="B41" s="141"/>
       <c r="C41" s="142"/>
       <c r="D41" s="142"/>
@@ -4334,7 +4368,7 @@
       <c r="L41" s="142"/>
       <c r="M41" s="142"/>
     </row>
-    <row r="42" spans="2:13" x14ac:dyDescent="0.2">
+    <row r="42" spans="2:13">
       <c r="B42" s="141"/>
       <c r="C42" s="142" t="s">
         <v>108</v>
@@ -4354,7 +4388,7 @@
       <c r="L42" s="142"/>
       <c r="M42" s="142"/>
     </row>
-    <row r="43" spans="2:13" x14ac:dyDescent="0.2">
+    <row r="43" spans="2:13">
       <c r="B43" s="141"/>
       <c r="C43" s="142" t="s">
         <v>105</v>
@@ -4374,7 +4408,7 @@
       <c r="L43" s="142"/>
       <c r="M43" s="142"/>
     </row>
-    <row r="44" spans="2:13" x14ac:dyDescent="0.2">
+    <row r="44" spans="2:13">
       <c r="B44" s="141"/>
       <c r="C44" s="142"/>
       <c r="D44" s="142"/>
@@ -4388,7 +4422,7 @@
       <c r="L44" s="142"/>
       <c r="M44" s="142"/>
     </row>
-    <row r="45" spans="2:13" x14ac:dyDescent="0.2">
+    <row r="45" spans="2:13">
       <c r="B45" s="141"/>
       <c r="C45" s="142"/>
       <c r="D45" s="142"/>
@@ -4402,7 +4436,7 @@
       <c r="L45" s="142"/>
       <c r="M45" s="142"/>
     </row>
-    <row r="46" spans="2:13" x14ac:dyDescent="0.2">
+    <row r="46" spans="2:13">
       <c r="B46" s="141"/>
       <c r="C46" s="142"/>
       <c r="D46" s="142"/>
@@ -4416,7 +4450,7 @@
       <c r="L46" s="142"/>
       <c r="M46" s="142"/>
     </row>
-    <row r="47" spans="2:13" x14ac:dyDescent="0.2">
+    <row r="47" spans="2:13">
       <c r="B47" s="141"/>
       <c r="C47" s="142"/>
       <c r="D47" s="142"/>
@@ -4430,7 +4464,7 @@
       <c r="L47" s="142"/>
       <c r="M47" s="142"/>
     </row>
-    <row r="48" spans="2:13" x14ac:dyDescent="0.2">
+    <row r="48" spans="2:13">
       <c r="B48" s="141"/>
       <c r="C48" s="142"/>
       <c r="D48" s="142"/>
@@ -4444,7 +4478,7 @@
       <c r="L48" s="142"/>
       <c r="M48" s="142"/>
     </row>
-    <row r="49" spans="2:13" x14ac:dyDescent="0.2">
+    <row r="49" spans="2:13">
       <c r="B49" s="141"/>
       <c r="C49" s="142"/>
       <c r="D49" s="142"/>
@@ -4458,7 +4492,7 @@
       <c r="L49" s="142"/>
       <c r="M49" s="142"/>
     </row>
-    <row r="50" spans="2:13" x14ac:dyDescent="0.2">
+    <row r="50" spans="2:13">
       <c r="B50" s="141"/>
       <c r="C50" s="142"/>
       <c r="D50" s="142"/>

</xml_diff>